<commit_message>
move the design change to each task; rewrite inference to sql; to be tested
</commit_message>
<xml_diff>
--- a/simcon.xlsx
+++ b/simcon.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="249" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="362" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="33">
   <si>
     <t>MeetingCycle</t>
   </si>
@@ -28,94 +28,97 @@
     <t>DesignChangeCycle</t>
   </si>
   <si>
+    <t>ProductionRateChange</t>
+  </si>
+  <si>
+    <t>QualityCheck</t>
+  </si>
+  <si>
+    <t>TaskSelectionFunction</t>
+  </si>
+  <si>
+    <t>PriorityChange</t>
+  </si>
+  <si>
+    <t>CollisionInformationExchnage</t>
+  </si>
+  <si>
+    <t>SubName</t>
+  </si>
+  <si>
+    <t>Electricity</t>
+  </si>
+  <si>
+    <t>Gravel</t>
+  </si>
+  <si>
+    <t>Partition</t>
+  </si>
+  <si>
+    <t>Plumbing</t>
+  </si>
+  <si>
+    <t>Tiling</t>
+  </si>
+  <si>
+    <t>WorkMethod</t>
+  </si>
+  <si>
+    <t>InitialProductionRate</t>
+  </si>
+  <si>
+    <t>QualityRate</t>
+  </si>
+  <si>
+    <t>PerformanceStd</t>
+  </si>
+  <si>
+    <t>Gravel base layer</t>
+  </si>
+  <si>
+    <t>Pipes in the floor</t>
+  </si>
+  <si>
+    <t>Electric conduits in the floor</t>
+  </si>
+  <si>
+    <t>Floor tiling</t>
+  </si>
+  <si>
+    <t>Partition phase 1</t>
+  </si>
+  <si>
+    <t>Pipes in the wall</t>
+  </si>
+  <si>
+    <t>Partition phase 2</t>
+  </si>
+  <si>
+    <t>Electric conduits in the wall</t>
+  </si>
+  <si>
+    <t>Partition phase 3</t>
+  </si>
+  <si>
+    <t>Wall tiling</t>
+  </si>
+  <si>
+    <t>PredecessorWorkMethod</t>
+  </si>
+  <si>
+    <t>SuccessorWorkMethod</t>
+  </si>
+  <si>
+    <t>Floor</t>
+  </si>
+  <si>
+    <t>InitialPriority</t>
+  </si>
+  <si>
+    <t>InitialQty</t>
+  </si>
+  <si>
     <t>DesignChangeVariation</t>
-  </si>
-  <si>
-    <t>ProductionRateChange</t>
-  </si>
-  <si>
-    <t>QualityCheck</t>
-  </si>
-  <si>
-    <t>TaskSelectionFunction</t>
-  </si>
-  <si>
-    <t>PriorityChange</t>
-  </si>
-  <si>
-    <t>SubName</t>
-  </si>
-  <si>
-    <t>Electricity</t>
-  </si>
-  <si>
-    <t>Gravel</t>
-  </si>
-  <si>
-    <t>Partition</t>
-  </si>
-  <si>
-    <t>Plumbing</t>
-  </si>
-  <si>
-    <t>Tiling</t>
-  </si>
-  <si>
-    <t>WorkMethod</t>
-  </si>
-  <si>
-    <t>InitialProductionRate</t>
-  </si>
-  <si>
-    <t>QualityRate</t>
-  </si>
-  <si>
-    <t>PerformanceStd</t>
-  </si>
-  <si>
-    <t>Gravel base layer</t>
-  </si>
-  <si>
-    <t>Pipes in the floor</t>
-  </si>
-  <si>
-    <t>Electric conduits in the floor</t>
-  </si>
-  <si>
-    <t>Floor tiling</t>
-  </si>
-  <si>
-    <t>Partition phase 1</t>
-  </si>
-  <si>
-    <t>Pipes in the wall</t>
-  </si>
-  <si>
-    <t>Partition phase 2</t>
-  </si>
-  <si>
-    <t>Electric conduits in the wall</t>
-  </si>
-  <si>
-    <t>Partition phase 3</t>
-  </si>
-  <si>
-    <t>Wall tiling</t>
-  </si>
-  <si>
-    <t>PredecessorWorkMethod</t>
-  </si>
-  <si>
-    <t>SuccessorWorkMethod</t>
-  </si>
-  <si>
-    <t>Floor</t>
-  </si>
-  <si>
-    <t>InitialPriority</t>
-  </si>
-  <si>
-    <t>InitialQty</t>
   </si>
 </sst>
 </file>
@@ -212,21 +215,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.5459183673469"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8265306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.1836734693878"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.0510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.4081632653061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.7704081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.3826530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.0510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4081632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.7704081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.3826530612245"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.469387755102"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
@@ -255,10 +258,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1</v>
@@ -267,59 +270,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F2" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="G2" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -398,7 +355,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -439,7 +396,7 @@
         <v>34</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>5</v>
@@ -456,7 +413,7 @@
         <v>69</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>5</v>
@@ -473,7 +430,7 @@
         <v>51</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>8</v>
@@ -490,7 +447,7 @@
         <v>62</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>9</v>
@@ -507,7 +464,7 @@
         <v>110</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>12</v>
@@ -524,7 +481,7 @@
         <v>37</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>9</v>
@@ -541,7 +498,7 @@
         <v>102</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>11</v>
@@ -558,7 +515,7 @@
         <v>41</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>2</v>
@@ -575,7 +532,7 @@
         <v>64</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>4</v>
@@ -592,7 +549,7 @@
         <v>27</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>2</v>
@@ -797,17 +754,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C42" activeCellId="0" sqref="C42"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.0714285714286"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.5969387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.79081632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.1836734693878"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -820,6 +779,9 @@
       <c r="C1" s="0" t="s">
         <v>31</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
@@ -831,6 +793,10 @@
       <c r="C2" s="0" t="n">
         <v>170</v>
       </c>
+      <c r="D2" s="0" t="n">
+        <f aca="false">0.1*C2</f>
+        <v>17</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
@@ -842,6 +808,10 @@
       <c r="C3" s="0" t="n">
         <v>100</v>
       </c>
+      <c r="D3" s="0" t="n">
+        <f aca="false">0.1*C3</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
@@ -853,6 +823,10 @@
       <c r="C4" s="0" t="n">
         <v>80</v>
       </c>
+      <c r="D4" s="0" t="n">
+        <f aca="false">0.1*C4</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
@@ -863,6 +837,10 @@
       </c>
       <c r="C5" s="0" t="n">
         <v>720</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <f aca="false">0.1*C5</f>
+        <v>72</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -875,6 +853,10 @@
       <c r="C6" s="0" t="n">
         <v>750</v>
       </c>
+      <c r="D6" s="0" t="n">
+        <f aca="false">0.1*C6</f>
+        <v>75</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -886,6 +868,10 @@
       <c r="C7" s="0" t="n">
         <v>190</v>
       </c>
+      <c r="D7" s="0" t="n">
+        <f aca="false">0.1*C7</f>
+        <v>19</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
@@ -897,6 +883,10 @@
       <c r="C8" s="0" t="n">
         <v>20</v>
       </c>
+      <c r="D8" s="0" t="n">
+        <f aca="false">0.1*C8</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
@@ -908,6 +898,10 @@
       <c r="C9" s="0" t="n">
         <v>180</v>
       </c>
+      <c r="D9" s="0" t="n">
+        <f aca="false">0.1*C9</f>
+        <v>18</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
@@ -919,6 +913,10 @@
       <c r="C10" s="0" t="n">
         <v>200</v>
       </c>
+      <c r="D10" s="0" t="n">
+        <f aca="false">0.1*C10</f>
+        <v>20</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
@@ -930,6 +928,10 @@
       <c r="C11" s="0" t="n">
         <v>290</v>
       </c>
+      <c r="D11" s="0" t="n">
+        <f aca="false">0.1*C11</f>
+        <v>29</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
@@ -941,6 +943,10 @@
       <c r="C12" s="0" t="n">
         <v>170</v>
       </c>
+      <c r="D12" s="0" t="n">
+        <f aca="false">0.1*C12</f>
+        <v>17</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
@@ -952,6 +958,10 @@
       <c r="C13" s="0" t="n">
         <v>100</v>
       </c>
+      <c r="D13" s="0" t="n">
+        <f aca="false">0.1*C13</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
@@ -963,6 +973,10 @@
       <c r="C14" s="0" t="n">
         <v>80</v>
       </c>
+      <c r="D14" s="0" t="n">
+        <f aca="false">0.1*C14</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
@@ -973,6 +987,10 @@
       </c>
       <c r="C15" s="0" t="n">
         <v>720</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <f aca="false">0.1*C15</f>
+        <v>72</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -985,6 +1003,10 @@
       <c r="C16" s="0" t="n">
         <v>750</v>
       </c>
+      <c r="D16" s="0" t="n">
+        <f aca="false">0.1*C16</f>
+        <v>75</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
@@ -996,6 +1018,10 @@
       <c r="C17" s="0" t="n">
         <v>190</v>
       </c>
+      <c r="D17" s="0" t="n">
+        <f aca="false">0.1*C17</f>
+        <v>19</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
@@ -1007,6 +1033,10 @@
       <c r="C18" s="0" t="n">
         <v>20</v>
       </c>
+      <c r="D18" s="0" t="n">
+        <f aca="false">0.1*C18</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
@@ -1018,6 +1048,10 @@
       <c r="C19" s="0" t="n">
         <v>180</v>
       </c>
+      <c r="D19" s="0" t="n">
+        <f aca="false">0.1*C19</f>
+        <v>18</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
@@ -1029,6 +1063,10 @@
       <c r="C20" s="0" t="n">
         <v>200</v>
       </c>
+      <c r="D20" s="0" t="n">
+        <f aca="false">0.1*C20</f>
+        <v>20</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
@@ -1040,6 +1078,10 @@
       <c r="C21" s="0" t="n">
         <v>290</v>
       </c>
+      <c r="D21" s="0" t="n">
+        <f aca="false">0.1*C21</f>
+        <v>29</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
@@ -1051,6 +1093,10 @@
       <c r="C22" s="0" t="n">
         <v>170</v>
       </c>
+      <c r="D22" s="0" t="n">
+        <f aca="false">0.1*C22</f>
+        <v>17</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
@@ -1062,6 +1108,10 @@
       <c r="C23" s="0" t="n">
         <v>100</v>
       </c>
+      <c r="D23" s="0" t="n">
+        <f aca="false">0.1*C23</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
@@ -1073,6 +1123,10 @@
       <c r="C24" s="0" t="n">
         <v>80</v>
       </c>
+      <c r="D24" s="0" t="n">
+        <f aca="false">0.1*C24</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
@@ -1083,6 +1137,10 @@
       </c>
       <c r="C25" s="0" t="n">
         <v>720</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <f aca="false">0.1*C25</f>
+        <v>72</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1095,6 +1153,10 @@
       <c r="C26" s="0" t="n">
         <v>750</v>
       </c>
+      <c r="D26" s="0" t="n">
+        <f aca="false">0.1*C26</f>
+        <v>75</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
@@ -1106,6 +1168,10 @@
       <c r="C27" s="0" t="n">
         <v>190</v>
       </c>
+      <c r="D27" s="0" t="n">
+        <f aca="false">0.1*C27</f>
+        <v>19</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
@@ -1117,6 +1183,10 @@
       <c r="C28" s="0" t="n">
         <v>20</v>
       </c>
+      <c r="D28" s="0" t="n">
+        <f aca="false">0.1*C28</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
@@ -1128,6 +1198,10 @@
       <c r="C29" s="0" t="n">
         <v>180</v>
       </c>
+      <c r="D29" s="0" t="n">
+        <f aca="false">0.1*C29</f>
+        <v>18</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
@@ -1139,6 +1213,10 @@
       <c r="C30" s="0" t="n">
         <v>200</v>
       </c>
+      <c r="D30" s="0" t="n">
+        <f aca="false">0.1*C30</f>
+        <v>20</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
@@ -1150,6 +1228,10 @@
       <c r="C31" s="0" t="n">
         <v>290</v>
       </c>
+      <c r="D31" s="0" t="n">
+        <f aca="false">0.1*C31</f>
+        <v>29</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
@@ -1161,6 +1243,10 @@
       <c r="C32" s="0" t="n">
         <v>170</v>
       </c>
+      <c r="D32" s="0" t="n">
+        <f aca="false">0.1*C32</f>
+        <v>17</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
@@ -1172,6 +1258,10 @@
       <c r="C33" s="0" t="n">
         <v>100</v>
       </c>
+      <c r="D33" s="0" t="n">
+        <f aca="false">0.1*C33</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
@@ -1183,6 +1273,10 @@
       <c r="C34" s="0" t="n">
         <v>80</v>
       </c>
+      <c r="D34" s="0" t="n">
+        <f aca="false">0.1*C34</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
@@ -1193,6 +1287,10 @@
       </c>
       <c r="C35" s="0" t="n">
         <v>720</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <f aca="false">0.1*C35</f>
+        <v>72</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1205,6 +1303,10 @@
       <c r="C36" s="0" t="n">
         <v>750</v>
       </c>
+      <c r="D36" s="0" t="n">
+        <f aca="false">0.1*C36</f>
+        <v>75</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
@@ -1216,6 +1318,10 @@
       <c r="C37" s="0" t="n">
         <v>190</v>
       </c>
+      <c r="D37" s="0" t="n">
+        <f aca="false">0.1*C37</f>
+        <v>19</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
@@ -1227,6 +1333,10 @@
       <c r="C38" s="0" t="n">
         <v>20</v>
       </c>
+      <c r="D38" s="0" t="n">
+        <f aca="false">0.1*C38</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
@@ -1238,6 +1348,10 @@
       <c r="C39" s="0" t="n">
         <v>180</v>
       </c>
+      <c r="D39" s="0" t="n">
+        <f aca="false">0.1*C39</f>
+        <v>18</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
@@ -1249,6 +1363,10 @@
       <c r="C40" s="0" t="n">
         <v>200</v>
       </c>
+      <c r="D40" s="0" t="n">
+        <f aca="false">0.1*C40</f>
+        <v>20</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
@@ -1260,6 +1378,10 @@
       <c r="C41" s="0" t="n">
         <v>290</v>
       </c>
+      <c r="D41" s="0" t="n">
+        <f aca="false">0.1*C41</f>
+        <v>29</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
@@ -1271,6 +1393,10 @@
       <c r="C42" s="0" t="n">
         <v>170</v>
       </c>
+      <c r="D42" s="0" t="n">
+        <f aca="false">0.1*C42</f>
+        <v>17</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
@@ -1282,6 +1408,10 @@
       <c r="C43" s="0" t="n">
         <v>100</v>
       </c>
+      <c r="D43" s="0" t="n">
+        <f aca="false">0.1*C43</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
@@ -1293,6 +1423,10 @@
       <c r="C44" s="0" t="n">
         <v>80</v>
       </c>
+      <c r="D44" s="0" t="n">
+        <f aca="false">0.1*C44</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
@@ -1303,6 +1437,10 @@
       </c>
       <c r="C45" s="0" t="n">
         <v>720</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <f aca="false">0.1*C45</f>
+        <v>72</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1315,6 +1453,10 @@
       <c r="C46" s="0" t="n">
         <v>750</v>
       </c>
+      <c r="D46" s="0" t="n">
+        <f aca="false">0.1*C46</f>
+        <v>75</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
@@ -1326,6 +1468,10 @@
       <c r="C47" s="0" t="n">
         <v>190</v>
       </c>
+      <c r="D47" s="0" t="n">
+        <f aca="false">0.1*C47</f>
+        <v>19</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
@@ -1337,6 +1483,10 @@
       <c r="C48" s="0" t="n">
         <v>20</v>
       </c>
+      <c r="D48" s="0" t="n">
+        <f aca="false">0.1*C48</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
@@ -1348,6 +1498,10 @@
       <c r="C49" s="0" t="n">
         <v>180</v>
       </c>
+      <c r="D49" s="0" t="n">
+        <f aca="false">0.1*C49</f>
+        <v>18</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
@@ -1359,6 +1513,10 @@
       <c r="C50" s="0" t="n">
         <v>200</v>
       </c>
+      <c r="D50" s="0" t="n">
+        <f aca="false">0.1*C50</f>
+        <v>20</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
@@ -1369,6 +1527,10 @@
       </c>
       <c r="C51" s="0" t="n">
         <v>290</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <f aca="false">0.1*C51</f>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix the inference bug, export quality check and design change(variation per task)
</commit_message>
<xml_diff>
--- a/simcon.xlsx
+++ b/simcon.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="362" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="362" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" state="visible" r:id="rId2"/>
@@ -217,8 +217,8 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="D2:D11 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -298,7 +298,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D2:D11 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -354,8 +354,8 @@
   </sheetPr>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -396,7 +396,7 @@
         <v>34</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>5</v>
@@ -413,7 +413,7 @@
         <v>69</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>5</v>
@@ -430,7 +430,7 @@
         <v>51</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>8</v>
@@ -447,7 +447,7 @@
         <v>62</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>9</v>
@@ -464,7 +464,7 @@
         <v>110</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>12</v>
@@ -481,7 +481,7 @@
         <v>37</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>9</v>
@@ -498,7 +498,7 @@
         <v>102</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>11</v>
@@ -515,7 +515,7 @@
         <v>41</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>2</v>
@@ -532,7 +532,7 @@
         <v>64</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>4</v>
@@ -549,7 +549,7 @@
         <v>27</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>2</v>
@@ -574,7 +574,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="D2:D11 B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -682,7 +682,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D2:D11 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -757,7 +757,7 @@
   <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="1" sqref="D2:D11 C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
add more rich info like waste, addvalue, etc.
</commit_message>
<xml_diff>
--- a/simcon.xlsx
+++ b/simcon.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="362" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="362" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" state="visible" r:id="rId2"/>
@@ -40,7 +40,7 @@
     <t>PriorityChange</t>
   </si>
   <si>
-    <t>CollisionInformationExchnage</t>
+    <t>CollisionInformationExchange</t>
   </si>
   <si>
     <t>SubName</t>
@@ -215,10 +215,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="D2:D11 A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -258,7 +258,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>30</v>
@@ -276,6 +276,75 @@
         <v>0</v>
       </c>
       <c r="G2" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -298,7 +367,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D2:D11 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -354,8 +423,8 @@
   </sheetPr>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2:D11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -393,13 +462,13 @@
         <v>17</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>0.9</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>5</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -410,13 +479,13 @@
         <v>18</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>69</v>
+        <v>1</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>0.9</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>5</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -427,13 +496,13 @@
         <v>19</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>51</v>
+        <v>1</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>0.9</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>8</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -444,13 +513,13 @@
         <v>20</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>62</v>
+        <v>1</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>0.9</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>9</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -461,13 +530,13 @@
         <v>21</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>110</v>
+        <v>1</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>0.9</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>12</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -478,13 +547,13 @@
         <v>22</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>0.9</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>9</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -495,13 +564,13 @@
         <v>23</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>102</v>
+        <v>1</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>0.9</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>11</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -512,13 +581,13 @@
         <v>24</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>0.9</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -529,13 +598,13 @@
         <v>25</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>64</v>
+        <v>1</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>0.9</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>4</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -546,13 +615,13 @@
         <v>26</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>0.9</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>2</v>
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>
@@ -574,7 +643,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="D2:D11 B6"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -682,7 +751,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D2:D11 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -757,7 +826,7 @@
   <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="1" sqref="D2:D11 C4"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -791,11 +860,11 @@
         <v>1</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>170</v>
+        <v>5</v>
       </c>
       <c r="D2" s="0" t="n">
         <f aca="false">0.1*C2</f>
-        <v>17</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -806,11 +875,11 @@
         <v>1</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="D3" s="0" t="n">
         <f aca="false">0.1*C3</f>
-        <v>10</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -821,11 +890,11 @@
         <v>1</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>80</v>
+        <v>5</v>
       </c>
       <c r="D4" s="0" t="n">
         <f aca="false">0.1*C4</f>
-        <v>8</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -836,11 +905,11 @@
         <v>1</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>720</v>
+        <v>5</v>
       </c>
       <c r="D5" s="0" t="n">
         <f aca="false">0.1*C5</f>
-        <v>72</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -851,11 +920,11 @@
         <v>1</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>750</v>
+        <v>5</v>
       </c>
       <c r="D6" s="0" t="n">
         <f aca="false">0.1*C6</f>
-        <v>75</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -866,11 +935,11 @@
         <v>1</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>190</v>
+        <v>5</v>
       </c>
       <c r="D7" s="0" t="n">
         <f aca="false">0.1*C7</f>
-        <v>19</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -881,11 +950,11 @@
         <v>1</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D8" s="0" t="n">
         <f aca="false">0.1*C8</f>
-        <v>2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -896,11 +965,11 @@
         <v>1</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>180</v>
+        <v>5</v>
       </c>
       <c r="D9" s="0" t="n">
         <f aca="false">0.1*C9</f>
-        <v>18</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -911,11 +980,11 @@
         <v>1</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>200</v>
+        <v>5</v>
       </c>
       <c r="D10" s="0" t="n">
         <f aca="false">0.1*C10</f>
-        <v>20</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -926,11 +995,11 @@
         <v>1</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>290</v>
+        <v>5</v>
       </c>
       <c r="D11" s="0" t="n">
         <f aca="false">0.1*C11</f>
-        <v>29</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -941,11 +1010,11 @@
         <v>2</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>170</v>
+        <v>5</v>
       </c>
       <c r="D12" s="0" t="n">
         <f aca="false">0.1*C12</f>
-        <v>17</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -956,11 +1025,11 @@
         <v>2</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="D13" s="0" t="n">
         <f aca="false">0.1*C13</f>
-        <v>10</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -971,11 +1040,11 @@
         <v>2</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>80</v>
+        <v>5</v>
       </c>
       <c r="D14" s="0" t="n">
         <f aca="false">0.1*C14</f>
-        <v>8</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -986,11 +1055,11 @@
         <v>2</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>720</v>
+        <v>5</v>
       </c>
       <c r="D15" s="0" t="n">
         <f aca="false">0.1*C15</f>
-        <v>72</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1001,11 +1070,11 @@
         <v>2</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>750</v>
+        <v>5</v>
       </c>
       <c r="D16" s="0" t="n">
         <f aca="false">0.1*C16</f>
-        <v>75</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1016,11 +1085,11 @@
         <v>2</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>190</v>
+        <v>5</v>
       </c>
       <c r="D17" s="0" t="n">
         <f aca="false">0.1*C17</f>
-        <v>19</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1031,11 +1100,11 @@
         <v>2</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D18" s="0" t="n">
         <f aca="false">0.1*C18</f>
-        <v>2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1046,11 +1115,11 @@
         <v>2</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>180</v>
+        <v>5</v>
       </c>
       <c r="D19" s="0" t="n">
         <f aca="false">0.1*C19</f>
-        <v>18</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1061,11 +1130,11 @@
         <v>2</v>
       </c>
       <c r="C20" s="0" t="n">
-        <v>200</v>
+        <v>5</v>
       </c>
       <c r="D20" s="0" t="n">
         <f aca="false">0.1*C20</f>
-        <v>20</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1076,11 +1145,11 @@
         <v>2</v>
       </c>
       <c r="C21" s="0" t="n">
-        <v>290</v>
+        <v>5</v>
       </c>
       <c r="D21" s="0" t="n">
         <f aca="false">0.1*C21</f>
-        <v>29</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1091,11 +1160,11 @@
         <v>3</v>
       </c>
       <c r="C22" s="0" t="n">
-        <v>170</v>
+        <v>5</v>
       </c>
       <c r="D22" s="0" t="n">
         <f aca="false">0.1*C22</f>
-        <v>17</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1106,11 +1175,11 @@
         <v>3</v>
       </c>
       <c r="C23" s="0" t="n">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="D23" s="0" t="n">
         <f aca="false">0.1*C23</f>
-        <v>10</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1121,11 +1190,11 @@
         <v>3</v>
       </c>
       <c r="C24" s="0" t="n">
-        <v>80</v>
+        <v>5</v>
       </c>
       <c r="D24" s="0" t="n">
         <f aca="false">0.1*C24</f>
-        <v>8</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1136,11 +1205,11 @@
         <v>3</v>
       </c>
       <c r="C25" s="0" t="n">
-        <v>720</v>
+        <v>5</v>
       </c>
       <c r="D25" s="0" t="n">
         <f aca="false">0.1*C25</f>
-        <v>72</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1151,11 +1220,11 @@
         <v>3</v>
       </c>
       <c r="C26" s="0" t="n">
-        <v>750</v>
+        <v>5</v>
       </c>
       <c r="D26" s="0" t="n">
         <f aca="false">0.1*C26</f>
-        <v>75</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1166,11 +1235,11 @@
         <v>3</v>
       </c>
       <c r="C27" s="0" t="n">
-        <v>190</v>
+        <v>5</v>
       </c>
       <c r="D27" s="0" t="n">
         <f aca="false">0.1*C27</f>
-        <v>19</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1181,11 +1250,11 @@
         <v>3</v>
       </c>
       <c r="C28" s="0" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D28" s="0" t="n">
         <f aca="false">0.1*C28</f>
-        <v>2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1196,11 +1265,11 @@
         <v>3</v>
       </c>
       <c r="C29" s="0" t="n">
-        <v>180</v>
+        <v>5</v>
       </c>
       <c r="D29" s="0" t="n">
         <f aca="false">0.1*C29</f>
-        <v>18</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1211,11 +1280,11 @@
         <v>3</v>
       </c>
       <c r="C30" s="0" t="n">
-        <v>200</v>
+        <v>5</v>
       </c>
       <c r="D30" s="0" t="n">
         <f aca="false">0.1*C30</f>
-        <v>20</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1226,11 +1295,11 @@
         <v>3</v>
       </c>
       <c r="C31" s="0" t="n">
-        <v>290</v>
+        <v>5</v>
       </c>
       <c r="D31" s="0" t="n">
         <f aca="false">0.1*C31</f>
-        <v>29</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1241,11 +1310,11 @@
         <v>4</v>
       </c>
       <c r="C32" s="0" t="n">
-        <v>170</v>
+        <v>5</v>
       </c>
       <c r="D32" s="0" t="n">
         <f aca="false">0.1*C32</f>
-        <v>17</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1256,11 +1325,11 @@
         <v>4</v>
       </c>
       <c r="C33" s="0" t="n">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="D33" s="0" t="n">
         <f aca="false">0.1*C33</f>
-        <v>10</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1271,11 +1340,11 @@
         <v>4</v>
       </c>
       <c r="C34" s="0" t="n">
-        <v>80</v>
+        <v>5</v>
       </c>
       <c r="D34" s="0" t="n">
         <f aca="false">0.1*C34</f>
-        <v>8</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1286,11 +1355,11 @@
         <v>4</v>
       </c>
       <c r="C35" s="0" t="n">
-        <v>720</v>
+        <v>5</v>
       </c>
       <c r="D35" s="0" t="n">
         <f aca="false">0.1*C35</f>
-        <v>72</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1301,11 +1370,11 @@
         <v>4</v>
       </c>
       <c r="C36" s="0" t="n">
-        <v>750</v>
+        <v>5</v>
       </c>
       <c r="D36" s="0" t="n">
         <f aca="false">0.1*C36</f>
-        <v>75</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1316,11 +1385,11 @@
         <v>4</v>
       </c>
       <c r="C37" s="0" t="n">
-        <v>190</v>
+        <v>5</v>
       </c>
       <c r="D37" s="0" t="n">
         <f aca="false">0.1*C37</f>
-        <v>19</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1331,11 +1400,11 @@
         <v>4</v>
       </c>
       <c r="C38" s="0" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D38" s="0" t="n">
         <f aca="false">0.1*C38</f>
-        <v>2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1346,11 +1415,11 @@
         <v>4</v>
       </c>
       <c r="C39" s="0" t="n">
-        <v>180</v>
+        <v>5</v>
       </c>
       <c r="D39" s="0" t="n">
         <f aca="false">0.1*C39</f>
-        <v>18</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1361,11 +1430,11 @@
         <v>4</v>
       </c>
       <c r="C40" s="0" t="n">
-        <v>200</v>
+        <v>5</v>
       </c>
       <c r="D40" s="0" t="n">
         <f aca="false">0.1*C40</f>
-        <v>20</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1376,11 +1445,11 @@
         <v>4</v>
       </c>
       <c r="C41" s="0" t="n">
-        <v>290</v>
+        <v>5</v>
       </c>
       <c r="D41" s="0" t="n">
         <f aca="false">0.1*C41</f>
-        <v>29</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1391,11 +1460,11 @@
         <v>5</v>
       </c>
       <c r="C42" s="0" t="n">
-        <v>170</v>
+        <v>5</v>
       </c>
       <c r="D42" s="0" t="n">
         <f aca="false">0.1*C42</f>
-        <v>17</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1406,11 +1475,11 @@
         <v>5</v>
       </c>
       <c r="C43" s="0" t="n">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="D43" s="0" t="n">
         <f aca="false">0.1*C43</f>
-        <v>10</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1421,11 +1490,11 @@
         <v>5</v>
       </c>
       <c r="C44" s="0" t="n">
-        <v>80</v>
+        <v>5</v>
       </c>
       <c r="D44" s="0" t="n">
         <f aca="false">0.1*C44</f>
-        <v>8</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1436,11 +1505,11 @@
         <v>5</v>
       </c>
       <c r="C45" s="0" t="n">
-        <v>720</v>
+        <v>5</v>
       </c>
       <c r="D45" s="0" t="n">
         <f aca="false">0.1*C45</f>
-        <v>72</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1451,11 +1520,11 @@
         <v>5</v>
       </c>
       <c r="C46" s="0" t="n">
-        <v>750</v>
+        <v>5</v>
       </c>
       <c r="D46" s="0" t="n">
         <f aca="false">0.1*C46</f>
-        <v>75</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1466,11 +1535,11 @@
         <v>5</v>
       </c>
       <c r="C47" s="0" t="n">
-        <v>190</v>
+        <v>5</v>
       </c>
       <c r="D47" s="0" t="n">
         <f aca="false">0.1*C47</f>
-        <v>19</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1481,11 +1550,11 @@
         <v>5</v>
       </c>
       <c r="C48" s="0" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D48" s="0" t="n">
         <f aca="false">0.1*C48</f>
-        <v>2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1496,11 +1565,11 @@
         <v>5</v>
       </c>
       <c r="C49" s="0" t="n">
-        <v>180</v>
+        <v>5</v>
       </c>
       <c r="D49" s="0" t="n">
         <f aca="false">0.1*C49</f>
-        <v>18</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1511,11 +1580,11 @@
         <v>5</v>
       </c>
       <c r="C50" s="0" t="n">
-        <v>200</v>
+        <v>5</v>
       </c>
       <c r="D50" s="0" t="n">
         <f aca="false">0.1*C50</f>
-        <v>20</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1526,11 +1595,11 @@
         <v>5</v>
       </c>
       <c r="C51" s="0" t="n">
-        <v>290</v>
+        <v>5</v>
       </c>
       <c r="D51" s="0" t="n">
         <f aca="false">0.1*C51</f>
-        <v>29</v>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add epic2.1 mysql version
</commit_message>
<xml_diff>
--- a/simcon.xlsx
+++ b/simcon.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="362" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="352" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="33">
   <si>
     <t>MeetingCycle</t>
   </si>
@@ -58,6 +58,9 @@
     <t>Tiling</t>
   </si>
   <si>
+    <t>Partition</t>
+  </si>
+  <si>
     <t>WorkMethod</t>
   </si>
   <si>
@@ -80,6 +83,24 @@
   </si>
   <si>
     <t>Floor tiling</t>
+  </si>
+  <si>
+    <t>Partition phase 1</t>
+  </si>
+  <si>
+    <t>Pipes in the wall</t>
+  </si>
+  <si>
+    <t>Electric conduits in the wall</t>
+  </si>
+  <si>
+    <t>Partition phase 2</t>
+  </si>
+  <si>
+    <t>Wall tiling</t>
+  </si>
+  <si>
+    <t>Partition phase 3</t>
   </si>
   <si>
     <t>PredecessorWorkMethod</t>
@@ -194,10 +215,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="1" sqref="C2:C51 A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -246,7 +267,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>1</v>
@@ -260,7 +281,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>10</v>
@@ -269,7 +290,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>1</v>
@@ -278,6 +299,75 @@
         <v>0</v>
       </c>
       <c r="G3" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -297,10 +387,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="1" sqref="C2:C51 A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -331,6 +421,11 @@
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -349,10 +444,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="C2:C51 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -370,16 +465,16 @@
         <v>7</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -387,16 +482,16 @@
         <v>9</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>0.1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -404,16 +499,16 @@
         <v>10</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>1</v>
+        <v>69</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>0.1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -421,16 +516,16 @@
         <v>8</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>0.1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -438,16 +533,118 @@
         <v>11</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>1</v>
+        <v>62</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>0.1</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -466,10 +663,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="C2:C51 B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -480,42 +677,82 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -537,7 +774,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C2:C51 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -547,10 +784,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -609,10 +846,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2:C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -626,316 +863,766 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>5</v>
+        <v>170</v>
       </c>
       <c r="D2" s="0" t="n">
         <f aca="false">0.1*C2</f>
-        <v>0.5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="D3" s="0" t="n">
         <f aca="false">0.1*C3</f>
-        <v>0.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>5</v>
+        <v>80</v>
       </c>
       <c r="D4" s="0" t="n">
         <f aca="false">0.1*C4</f>
-        <v>0.5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>5</v>
+        <v>720</v>
       </c>
       <c r="D5" s="0" t="n">
         <f aca="false">0.1*C5</f>
-        <v>0.5</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>5</v>
+        <v>750</v>
       </c>
       <c r="D6" s="0" t="n">
         <f aca="false">0.1*C6</f>
-        <v>0.5</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>5</v>
+        <v>190</v>
       </c>
       <c r="D7" s="0" t="n">
         <f aca="false">0.1*C7</f>
-        <v>0.5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>5</v>
+        <v>180</v>
       </c>
       <c r="D8" s="0" t="n">
         <f aca="false">0.1*C8</f>
-        <v>0.5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D9" s="0" t="n">
         <f aca="false">0.1*C9</f>
-        <v>0.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>5</v>
+        <v>290</v>
       </c>
       <c r="D10" s="0" t="n">
         <f aca="false">0.1*C10</f>
-        <v>0.5</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>5</v>
+        <v>200</v>
       </c>
       <c r="D11" s="0" t="n">
         <f aca="false">0.1*C11</f>
-        <v>0.5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>5</v>
+        <v>170</v>
       </c>
       <c r="D12" s="0" t="n">
         <f aca="false">0.1*C12</f>
-        <v>0.5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="D13" s="0" t="n">
         <f aca="false">0.1*C13</f>
-        <v>0.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>5</v>
+        <v>80</v>
       </c>
       <c r="D14" s="0" t="n">
         <f aca="false">0.1*C14</f>
-        <v>0.5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>5</v>
+        <v>720</v>
       </c>
       <c r="D15" s="0" t="n">
         <f aca="false">0.1*C15</f>
-        <v>0.5</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>5</v>
+        <v>750</v>
       </c>
       <c r="D16" s="0" t="n">
         <f aca="false">0.1*C16</f>
-        <v>0.5</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>5</v>
+        <v>190</v>
       </c>
       <c r="D17" s="0" t="n">
         <f aca="false">0.1*C17</f>
-        <v>0.5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>5</v>
+        <v>180</v>
       </c>
       <c r="D18" s="0" t="n">
         <f aca="false">0.1*C18</f>
-        <v>0.5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D19" s="0" t="n">
         <f aca="false">0.1*C19</f>
-        <v>0.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C20" s="0" t="n">
-        <v>5</v>
+        <v>290</v>
       </c>
       <c r="D20" s="0" t="n">
         <f aca="false">0.1*C20</f>
-        <v>0.5</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C21" s="0" t="n">
-        <v>5</v>
+        <v>200</v>
       </c>
       <c r="D21" s="0" t="n">
         <f aca="false">0.1*C21</f>
-        <v>0.5</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>170</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <f aca="false">0.1*C22</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <f aca="false">0.1*C23</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <f aca="false">0.1*C24</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>720</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <f aca="false">0.1*C25</f>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <f aca="false">0.1*C26</f>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>190</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <f aca="false">0.1*C27</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>180</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <f aca="false">0.1*C28</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <f aca="false">0.1*C29</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>290</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <f aca="false">0.1*C30</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <f aca="false">0.1*C31</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>170</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <f aca="false">0.1*C32</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <f aca="false">0.1*C33</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <f aca="false">0.1*C34</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>720</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <f aca="false">0.1*C35</f>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <f aca="false">0.1*C36</f>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>190</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <f aca="false">0.1*C37</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>180</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <f aca="false">0.1*C38</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <f aca="false">0.1*C39</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>290</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <f aca="false">0.1*C40</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <f aca="false">0.1*C41</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>170</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <f aca="false">0.1*C42</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <f aca="false">0.1*C43</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <f aca="false">0.1*C44</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>720</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <f aca="false">0.1*C45</f>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <f aca="false">0.1*C46</f>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C47" s="0" t="n">
+        <v>190</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <f aca="false">0.1*C47</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C48" s="0" t="n">
+        <v>180</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <f aca="false">0.1*C48</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B49" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <f aca="false">0.1*C49</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B50" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C50" s="0" t="n">
+        <v>290</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <f aca="false">0.1*C50</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B51" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C51" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <f aca="false">0.1*C51</f>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>